<commit_message>
Added selecting different browser versions capability.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbakheet/IdeaProjects/Selenium-TestNG-DDT-Framework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607AAB17-1303-E447-A9A4-9C57DCF4544B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E665012-D127-EA4F-AA2F-318834E909A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="500" windowWidth="30160" windowHeight="18840" activeTab="1" xr2:uid="{C09FCC8E-6533-D04F-8E2B-73F08B6B6705}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>testname</t>
   </si>
@@ -72,40 +72,49 @@
     <t>2</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>ScubaDrew615</t>
+  </si>
+  <si>
+    <t>admin12</t>
+  </si>
+  <si>
+    <t>To check whether the user can unsuccessfully login and out</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>79.0.3945.117</t>
+  </si>
+  <si>
+    <t>94.0.4606.61</t>
+  </si>
+  <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>Admin123</t>
-  </si>
-  <si>
-    <t>ScubaDrew615</t>
-  </si>
-  <si>
-    <t>admin12</t>
-  </si>
-  <si>
-    <t>To check whether the user can unsuccessfully login and out</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -516,7 +525,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -536,22 +545,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F217D9F-50A4-0943-B85D-60BBE4F89549}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,19 +570,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -579,39 +593,45 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -619,50 +639,53 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the excel sheet on work computer
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbakheet/IdeaProjects/Selenium-Framework/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BNAJWGuest.TBA-JWN-D077E9G\IdeaProjects\SeleniumFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481B35D5-EAA1-1449-8DA8-909274455845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18840" activeTab="1" xr2:uid="{C09FCC8E-6533-D04F-8E2B-73F08B6B6705}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -106,12 +105,15 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -462,19 +464,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08839DD-B4D5-2D41-B6DC-B2FDD8CD4344}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="223" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -535,20 +537,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F217D9F-50A4-0943-B85D-60BBE4F89549}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -579,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -619,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>

</xml_diff>